<commit_message>
add to cart bug fixed in product details page
</commit_message>
<xml_diff>
--- a/helpers/sales_report.xlsx
+++ b/helpers/sales_report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="48">
   <si>
     <t>SL No</t>
   </si>
@@ -43,28 +43,43 @@
     <t>Status</t>
   </si>
   <si>
-    <t>#ORD#27496852</t>
-  </si>
-  <si>
-    <t>salva</t>
-  </si>
-  <si>
-    <t>2025-05-20</t>
-  </si>
-  <si>
-    <t>Hive Full-Size Black - Purple Wired Gaming Keyboard</t>
+    <t>#ORD#47497504</t>
+  </si>
+  <si>
+    <t>cez</t>
+  </si>
+  <si>
+    <t>2025-06-02</t>
+  </si>
+  <si>
+    <t>Swarm All Black Wireless Gaming Keyboard</t>
+  </si>
+  <si>
+    <t>₹5,299</t>
+  </si>
+  <si>
+    <t>₹500</t>
+  </si>
+  <si>
+    <t>razorpay</t>
+  </si>
+  <si>
+    <t>Delivered</t>
+  </si>
+  <si>
+    <t>#ORD#33233257</t>
+  </si>
+  <si>
+    <t>Hive Full-Size White - Purple Wired Gaming Keyboard</t>
   </si>
   <si>
     <t>₹3,199</t>
   </si>
   <si>
-    <t>₹0</t>
-  </si>
-  <si>
-    <t>razorpay</t>
-  </si>
-  <si>
-    <t>Delivered</t>
+    <t>₹100</t>
+  </si>
+  <si>
+    <t>#ORD#84973799</t>
   </si>
   <si>
     <t>Hive Black - Purple Wired Gaming Keyboard</t>
@@ -73,7 +88,19 @@
     <t>₹2,699</t>
   </si>
   <si>
-    <t>#ORD#74844055</t>
+    <t>#ORD#22689663</t>
+  </si>
+  <si>
+    <t>Hive Full-Size All White Wired Gaming Keyboard</t>
+  </si>
+  <si>
+    <t>₹3,149</t>
+  </si>
+  <si>
+    <t>#ORD#61719044</t>
+  </si>
+  <si>
+    <t>2025-06-03</t>
   </si>
   <si>
     <t>Hive 75</t>
@@ -82,45 +109,27 @@
     <t>₹2,799</t>
   </si>
   <si>
-    <t>#ORD#88793903</t>
-  </si>
-  <si>
-    <t>Swarm All Black Wireless Gaming Keyboard</t>
-  </si>
-  <si>
-    <t>₹5,299</t>
-  </si>
-  <si>
-    <t>₹500</t>
-  </si>
-  <si>
-    <t>Hive All White RGB Wired Gaming Keyboard</t>
+    <t>#ORD#39594894</t>
+  </si>
+  <si>
+    <t>Hive White-Purple Wired Gaming Keyboard GAMING</t>
+  </si>
+  <si>
+    <t>Placed</t>
+  </si>
+  <si>
+    <t>#ORD#99299019</t>
+  </si>
+  <si>
+    <t>2025-06-04</t>
+  </si>
+  <si>
+    <t>Hive All Black RGB Wired Gaming Keyboard</t>
   </si>
   <si>
     <t>₹2,649</t>
   </si>
   <si>
-    <t>#ORD#51798406</t>
-  </si>
-  <si>
-    <t>Devu Devu</t>
-  </si>
-  <si>
-    <t>Hive Full-Size All White Wired Gaming Keyboard</t>
-  </si>
-  <si>
-    <t>₹3,149</t>
-  </si>
-  <si>
-    <t>#ORD#24027091</t>
-  </si>
-  <si>
-    <t>Hive Full-Size All Black Wired Gaming Keyboard</t>
-  </si>
-  <si>
-    <t>₹100</t>
-  </si>
-  <si>
     <t>Summary:</t>
   </si>
   <si>
@@ -133,19 +142,19 @@
     <t>Total Amount (₹)</t>
   </si>
   <si>
-    <t>₹22,943</t>
+    <t>₹27,891</t>
   </si>
   <si>
     <t>Total Discounts (₹)</t>
   </si>
   <si>
-    <t>₹1,100</t>
+    <t>₹2,900</t>
   </si>
   <si>
     <t>Net Sales (₹)</t>
   </si>
   <si>
-    <t>₹21,843</t>
+    <t>₹24,991</t>
   </si>
 </sst>
 </file>
@@ -522,7 +531,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J15"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -605,7 +614,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -614,16 +623,16 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="I3" t="s">
         <v>16</v>
@@ -637,7 +646,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -646,16 +655,16 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
         <v>21</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" t="s">
-        <v>15</v>
       </c>
       <c r="I4" t="s">
         <v>16</v>
@@ -669,7 +678,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -678,16 +687,16 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H5" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="I5" t="s">
         <v>16</v>
@@ -701,25 +710,25 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="I6" t="s">
         <v>16</v>
@@ -733,22 +742,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
         <v>29</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>30</v>
       </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
         <v>31</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>32</v>
       </c>
       <c r="H7" t="s">
         <v>15</v>
@@ -765,75 +774,139 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
         <v>33</v>
       </c>
-      <c r="C8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>34</v>
-      </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="H8" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="I8" t="s">
         <v>16</v>
       </c>
       <c r="J8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
         <v>36</v>
       </c>
-      <c r="B10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" t="s">
-        <v>40</v>
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G12" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" t="s">
         <v>43</v>
       </c>
-      <c r="G13" t="s">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
         <v>44</v>
+      </c>
+      <c r="G14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sales report bug fixed 'refund'
</commit_message>
<xml_diff>
--- a/helpers/sales_report.xlsx
+++ b/helpers/sales_report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="65">
   <si>
     <t>SL No</t>
   </si>
@@ -43,91 +43,142 @@
     <t>Status</t>
   </si>
   <si>
-    <t>#ORD#47497504</t>
-  </si>
-  <si>
-    <t>cez</t>
-  </si>
-  <si>
-    <t>2025-06-02</t>
+    <t>#ORD#59355935</t>
+  </si>
+  <si>
+    <t>salva</t>
+  </si>
+  <si>
+    <t>2025-06-12</t>
+  </si>
+  <si>
+    <t>Hive All White RGB Wired Gaming Keyboard</t>
+  </si>
+  <si>
+    <t>₹2,649</t>
+  </si>
+  <si>
+    <t>₹500</t>
+  </si>
+  <si>
+    <t>razorpay</t>
+  </si>
+  <si>
+    <t>Placed</t>
+  </si>
+  <si>
+    <t>Hive Full-Size All White Wired Gaming Keyboard</t>
+  </si>
+  <si>
+    <t>₹3,149</t>
+  </si>
+  <si>
+    <t>Hive All Black RGB Wired Gaming Keyboard</t>
+  </si>
+  <si>
+    <t>#ORD#81944325</t>
+  </si>
+  <si>
+    <t>Hive Full-Size White - Purple Wired Gaming Keyboard</t>
+  </si>
+  <si>
+    <t>₹3,199</t>
+  </si>
+  <si>
+    <t>#ORD#30466437</t>
+  </si>
+  <si>
+    <t>₹0</t>
+  </si>
+  <si>
+    <t>wallet</t>
+  </si>
+  <si>
+    <t>Returned</t>
+  </si>
+  <si>
+    <t>#ORD#43444435</t>
   </si>
   <si>
     <t>Swarm All Black Wireless Gaming Keyboard</t>
   </si>
   <si>
+    <t>#ORD#96441979</t>
+  </si>
+  <si>
+    <t>#ORD#51523113</t>
+  </si>
+  <si>
+    <t>Swarm Black Purple Wireless Gaming Keyboard</t>
+  </si>
+  <si>
+    <t>Hive Black - Purple Wired Gaming Keyboard</t>
+  </si>
+  <si>
+    <t>Hive Full-Size Black - Purple Wired Gaming Keyboard</t>
+  </si>
+  <si>
+    <t>Rejected</t>
+  </si>
+  <si>
+    <t>#ORD#28054257</t>
+  </si>
+  <si>
+    <t>Cezanne P</t>
+  </si>
+  <si>
+    <t>Hive Full-Size All Black Wired Gaming Keyboard</t>
+  </si>
+  <si>
+    <t>#ORD#55464487</t>
+  </si>
+  <si>
+    <t>#ORD#44965605</t>
+  </si>
+  <si>
+    <t>#ORD#93073047</t>
+  </si>
+  <si>
+    <t>#ORD#60822902</t>
+  </si>
+  <si>
+    <t>#ORD#36027666</t>
+  </si>
+  <si>
+    <t>#ORD#25129159</t>
+  </si>
+  <si>
+    <t>Swarm All White Wireless Gaming Keyboard</t>
+  </si>
+  <si>
+    <t>#ORD#74195435</t>
+  </si>
+  <si>
+    <t>Delivered</t>
+  </si>
+  <si>
     <t>₹5,299</t>
   </si>
   <si>
-    <t>₹500</t>
-  </si>
-  <si>
-    <t>razorpay</t>
-  </si>
-  <si>
-    <t>Delivered</t>
-  </si>
-  <si>
-    <t>#ORD#33233257</t>
-  </si>
-  <si>
-    <t>Hive Full-Size White - Purple Wired Gaming Keyboard</t>
-  </si>
-  <si>
-    <t>₹3,199</t>
-  </si>
-  <si>
-    <t>₹100</t>
-  </si>
-  <si>
-    <t>#ORD#84973799</t>
-  </si>
-  <si>
-    <t>Hive Black - Purple Wired Gaming Keyboard</t>
-  </si>
-  <si>
     <t>₹2,699</t>
   </si>
   <si>
-    <t>#ORD#22689663</t>
-  </si>
-  <si>
-    <t>Hive Full-Size All White Wired Gaming Keyboard</t>
-  </si>
-  <si>
-    <t>₹3,149</t>
-  </si>
-  <si>
-    <t>#ORD#61719044</t>
-  </si>
-  <si>
-    <t>2025-06-03</t>
-  </si>
-  <si>
-    <t>Hive 75</t>
-  </si>
-  <si>
-    <t>₹2,799</t>
-  </si>
-  <si>
-    <t>#ORD#39594894</t>
+    <t>#ORD#70337860</t>
   </si>
   <si>
     <t>Hive White-Purple Wired Gaming Keyboard GAMING</t>
   </si>
   <si>
-    <t>Placed</t>
-  </si>
-  <si>
-    <t>#ORD#99299019</t>
-  </si>
-  <si>
-    <t>2025-06-04</t>
-  </si>
-  <si>
-    <t>Hive All Black RGB Wired Gaming Keyboard</t>
-  </si>
-  <si>
-    <t>₹2,649</t>
+    <t>#undefined</t>
+  </si>
+  <si>
+    <t>#ORD#61059653</t>
+  </si>
+  <si>
+    <t>#ORD#12023198</t>
+  </si>
+  <si>
+    <t>#ORD#95305272</t>
   </si>
   <si>
     <t>Summary:</t>
@@ -142,19 +193,19 @@
     <t>Total Amount (₹)</t>
   </si>
   <si>
-    <t>₹27,891</t>
+    <t>₹55,682</t>
   </si>
   <si>
     <t>Total Discounts (₹)</t>
   </si>
   <si>
-    <t>₹2,900</t>
+    <t>₹2,000</t>
   </si>
   <si>
     <t>Net Sales (₹)</t>
   </si>
   <si>
-    <t>₹24,991</t>
+    <t>₹53,682</t>
   </si>
 </sst>
 </file>
@@ -531,7 +582,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J43"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -614,25 +665,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>19</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="I3" t="s">
         <v>16</v>
@@ -646,7 +697,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -655,16 +706,16 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="I4" t="s">
         <v>16</v>
@@ -678,7 +729,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -687,13 +738,13 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
@@ -710,31 +761,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="I6" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="J6" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -748,25 +799,25 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
         <v>29</v>
       </c>
-      <c r="E7" t="s">
-        <v>30</v>
-      </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="I7" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="J7" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -774,31 +825,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="I8" t="s">
         <v>16</v>
       </c>
       <c r="J8" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -806,31 +857,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="H9" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="I9" t="s">
         <v>16</v>
       </c>
       <c r="J9" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -838,75 +889,971 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" t="s">
         <v>35</v>
       </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>36</v>
       </c>
-      <c r="E10" t="s">
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" t="s">
+        <v>16</v>
+      </c>
+      <c r="J14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" t="s">
+        <v>25</v>
+      </c>
+      <c r="I17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" t="s">
+        <v>16</v>
+      </c>
+      <c r="J18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" t="s">
+        <v>16</v>
+      </c>
+      <c r="J19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" t="s">
+        <v>25</v>
+      </c>
+      <c r="I20" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" t="s">
+        <v>25</v>
+      </c>
+      <c r="I21" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" t="s">
+        <v>25</v>
+      </c>
+      <c r="I23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>23</v>
       </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" t="s">
+        <v>25</v>
+      </c>
+      <c r="I24" t="s">
+        <v>16</v>
+      </c>
+      <c r="J24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>24</v>
       </c>
-      <c r="H10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" t="s">
-        <v>16</v>
-      </c>
-      <c r="J10" t="s">
+      <c r="B25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" t="s">
+        <v>25</v>
+      </c>
+      <c r="I25" t="s">
+        <v>16</v>
+      </c>
+      <c r="J25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" t="s">
+        <v>25</v>
+      </c>
+      <c r="I26" t="s">
+        <v>16</v>
+      </c>
+      <c r="J26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27" t="s">
+        <v>23</v>
+      </c>
+      <c r="H27" t="s">
+        <v>25</v>
+      </c>
+      <c r="I27" t="s">
+        <v>16</v>
+      </c>
+      <c r="J27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28" t="s">
+        <v>48</v>
+      </c>
+      <c r="H28" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28" t="s">
+        <v>16</v>
+      </c>
+      <c r="J28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29" t="s">
+        <v>49</v>
+      </c>
+      <c r="H29" t="s">
+        <v>25</v>
+      </c>
+      <c r="I29" t="s">
+        <v>16</v>
+      </c>
+      <c r="J29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30" t="s">
+        <v>19</v>
+      </c>
+      <c r="H30" t="s">
+        <v>25</v>
+      </c>
+      <c r="I30" t="s">
+        <v>16</v>
+      </c>
+      <c r="J30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" t="s">
+        <v>51</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31" t="s">
+        <v>25</v>
+      </c>
+      <c r="I31" t="s">
+        <v>16</v>
+      </c>
+      <c r="J31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32" t="s">
+        <v>14</v>
+      </c>
+      <c r="H32" t="s">
+        <v>25</v>
+      </c>
+      <c r="I32" t="s">
+        <v>16</v>
+      </c>
+      <c r="J32" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" t="s">
-        <v>46</v>
-      </c>
-      <c r="G15" t="s">
-        <v>47</v>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33" t="s">
+        <v>14</v>
+      </c>
+      <c r="H33" t="s">
+        <v>25</v>
+      </c>
+      <c r="I33" t="s">
+        <v>16</v>
+      </c>
+      <c r="J33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" t="s">
+        <v>22</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34" t="s">
+        <v>23</v>
+      </c>
+      <c r="H34" t="s">
+        <v>25</v>
+      </c>
+      <c r="I34" t="s">
+        <v>16</v>
+      </c>
+      <c r="J34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
+        <v>19</v>
+      </c>
+      <c r="H35" t="s">
+        <v>25</v>
+      </c>
+      <c r="I35" t="s">
+        <v>16</v>
+      </c>
+      <c r="J35" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" t="s">
+        <v>22</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36" t="s">
+        <v>23</v>
+      </c>
+      <c r="H36" t="s">
+        <v>25</v>
+      </c>
+      <c r="I36" t="s">
+        <v>16</v>
+      </c>
+      <c r="J36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" t="s">
+        <v>22</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37" t="s">
+        <v>23</v>
+      </c>
+      <c r="H37" t="s">
+        <v>25</v>
+      </c>
+      <c r="I37" t="s">
+        <v>26</v>
+      </c>
+      <c r="J37" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" t="s">
+        <v>22</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38" t="s">
+        <v>25</v>
+      </c>
+      <c r="H38" t="s">
+        <v>25</v>
+      </c>
+      <c r="I38" t="s">
+        <v>16</v>
+      </c>
+      <c r="J38" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" t="s">
+        <v>57</v>
+      </c>
+      <c r="G40">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41" t="s">
+        <v>59</v>
+      </c>
+      <c r="G41" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" t="s">
+        <v>61</v>
+      </c>
+      <c r="G42" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B43" t="s">
+        <v>63</v>
+      </c>
+      <c r="G43" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>